<commit_message>
added hooks and added secound test in progress
</commit_message>
<xml_diff>
--- a/testData/RetirementData.xlsx
+++ b/testData/RetirementData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehtis\Desktop\Project\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962930EE-2C8F-4C36-95A6-B836D2ED8C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3276F1-1B1B-4F02-A38D-18D020758F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{869F0F46-58A2-4284-9CED-E3D072A83001}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>current_age</t>
   </si>
@@ -46,13 +46,28 @@
   </si>
   <si>
     <t>savings_balance</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>SocialSecurityBenefits</t>
+  </si>
+  <si>
+    <t>maritalStatus</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>social_security_override</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +95,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -101,16 +123,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -427,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05C4333-5122-4DC2-96D2-2DD59E7B1194}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,32 +467,44 @@
     <col min="5" max="5" width="20.109375" customWidth="1"/>
     <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.44140625" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+    <col min="10" max="10" width="35.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>40</v>
       </c>
@@ -483,14 +520,23 @@
       <c r="E2" s="2">
         <v>500000</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2">
         <v>10</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="2">
         <v>2</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="2">
+        <v>14576</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="C3" s="1"/>
     </row>
   </sheetData>

</xml_diff>